<commit_message>
Excel error fixed. Everything is working correctly. No bugs
</commit_message>
<xml_diff>
--- a/excel_file/LCOH_Multi_Year.xlsx
+++ b/excel_file/LCOH_Multi_Year.xlsx
@@ -1,14 +1,34 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="present" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2030" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2050" sheetId="3" state="visible" r:id="rId3"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -19,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -27,12 +47,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +422,589 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22.8" customWidth="1" min="1" max="1"/>
+    <col width="8.4" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LCOH</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Solar PEM</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore PEM</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>14.13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore PEM</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear PEM</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Solar AWE</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>4.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AWE</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AWE</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AWE</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Solar SOEC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>8.449999999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore SOEC</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore SOEC</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear SOEC</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Solar AEM</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AEM</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>14.87</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AEM</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AEM</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>3.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22.8" customWidth="1" min="1" max="1"/>
+    <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LCOH</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Solar PEM</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore PEM</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore PEM</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear PEM</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Solar AWE</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AWE</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AWE</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AWE</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Solar SOEC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>9.449999999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore SOEC</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>9.630000000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore SOEC</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear SOEC</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Solar AEM</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AEM</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AEM</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AEM</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>5.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22.8" customWidth="1" min="1" max="1"/>
+    <col width="8.4" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LCOH</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Solar PEM</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>18.62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore PEM</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>14.52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore PEM</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>36.83</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear PEM</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Solar AWE</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>19.16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AWE</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AWE</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>38.42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AWE</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>28.72</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Solar SOEC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>19.49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore SOEC</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore SOEC</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>33.7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear SOEC</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>26.54</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Solar AEM</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>WindOnshore AEM</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>WindOffshore AEM</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>36.65</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Nuclear AEM</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>27.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>